<commit_message>
Fixed issue with order column, should be 2 columns: substrate order and product order
</commit_message>
<xml_diff>
--- a/set_up_grasp_models/tests/test_files/test_check_models/HMP2360_r0_t0.xlsx
+++ b/set_up_grasp_models/tests/test_files/test_check_models/HMP2360_r0_t0.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="8"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="1" state="visible" r:id="rId2"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="137">
   <si>
     <t>General Reaction and Sampling Platform (GRASP)</t>
   </si>
@@ -364,7 +364,10 @@
     <t>kinetic mechanism</t>
   </si>
   <si>
-    <t>order</t>
+    <t>substrate order</t>
+  </si>
+  <si>
+    <t>product order</t>
   </si>
   <si>
     <t>promiscuous</t>
@@ -559,7 +562,7 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D2:D7 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -692,7 +695,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D2:D7 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -838,7 +841,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D2:D7 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1061,7 +1064,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D2:D7 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1379,18 +1382,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K14"/>
+  <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2:D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.2591093117409"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.251012145749"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>108</v>
       </c>
@@ -1424,262 +1430,283 @@
       <c r="K1" s="1" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L1" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>39</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="E2" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="F2" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="I2" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="J2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="K2" s="0" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L2" s="0" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D3" s="0" t="s">
         <v>124</v>
       </c>
-      <c r="I3" s="0" t="n">
-        <v>0</v>
+      <c r="E3" s="0" t="s">
+        <v>125</v>
       </c>
       <c r="J3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="K3" s="0" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L3" s="0" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D4" s="0" t="s">
         <v>128</v>
       </c>
       <c r="E4" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="F4" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="I4" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="J4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="K4" s="0" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0</v>
+      </c>
+      <c r="K4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L4" s="0" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>42</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>131</v>
-      </c>
-      <c r="I5" s="0" t="n">
-        <v>0</v>
+        <v>132</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>132</v>
       </c>
       <c r="J5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="K5" s="0" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L5" s="0" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>43</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D6" s="0" t="s">
         <v>124</v>
       </c>
-      <c r="I6" s="0" t="n">
-        <v>0</v>
+      <c r="E6" s="0" t="s">
+        <v>125</v>
       </c>
       <c r="J6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="K6" s="0" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L6" s="0" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D7" s="0" t="s">
         <v>128</v>
       </c>
       <c r="E7" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="F7" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="I7" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="J7" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="K7" s="0" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0</v>
+      </c>
+      <c r="K7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L7" s="0" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>134</v>
-      </c>
-      <c r="I8" s="0" t="n">
-        <v>0</v>
+        <v>135</v>
       </c>
       <c r="J8" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0</v>
+      </c>
+      <c r="K8" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>134</v>
-      </c>
-      <c r="I9" s="0" t="n">
-        <v>0</v>
+        <v>135</v>
       </c>
       <c r="J9" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="K9" s="0" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0</v>
+      </c>
+      <c r="K9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L9" s="0" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
         <v>47</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>134</v>
-      </c>
-      <c r="I10" s="0" t="n">
-        <v>0</v>
+        <v>135</v>
       </c>
       <c r="J10" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="K10" s="0" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0</v>
+      </c>
+      <c r="K10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L10" s="0" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
         <v>48</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>134</v>
-      </c>
-      <c r="I11" s="0" t="n">
-        <v>0</v>
+        <v>135</v>
       </c>
       <c r="J11" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="K11" s="0" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0</v>
+      </c>
+      <c r="K11" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L11" s="0" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
         <v>49</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>134</v>
-      </c>
-      <c r="I12" s="0" t="n">
-        <v>0</v>
+        <v>135</v>
       </c>
       <c r="J12" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="K12" s="0" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0</v>
+      </c>
+      <c r="K12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L12" s="0" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
         <v>50</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>134</v>
-      </c>
-      <c r="I13" s="0" t="n">
-        <v>0</v>
+        <v>135</v>
       </c>
       <c r="J13" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="K13" s="0" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0</v>
+      </c>
+      <c r="K13" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L13" s="0" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
         <v>51</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>134</v>
-      </c>
-      <c r="I14" s="0" t="n">
-        <v>0</v>
+        <v>135</v>
       </c>
       <c r="J14" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="K14" s="0" t="s">
-        <v>135</v>
+        <v>0</v>
+      </c>
+      <c r="K14" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L14" s="0" t="s">
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -1701,7 +1728,7 @@
   <dimension ref="A1:U14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D2:D7 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2638,7 +2665,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D2:D7 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3022,7 +3049,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D2:D7 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3245,7 +3272,7 @@
   <dimension ref="A2:A15"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D2:D7 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3342,7 +3369,7 @@
   <dimension ref="A2:A22"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D2:D7 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3474,7 +3501,7 @@
   <dimension ref="A2:A22"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D2:D7 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3606,7 +3633,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="D2:D7 B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3786,8 +3813,8 @@
   </sheetPr>
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E17" activeCellId="1" sqref="D2:D7 E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Feat: when reading an excel file index_col=0 must be set, always.
The idea is to be consistent across the package
</commit_message>
<xml_diff>
--- a/set_up_grasp_models/tests/test_files/test_check_models/HMP2360_r0_t0.xlsx
+++ b/set_up_grasp_models/tests/test_files/test_check_models/HMP2360_r0_t0.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="12"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="1" state="visible" r:id="rId2"/>
@@ -328,16 +328,16 @@
     <t>Fluxes (umol/gCDW/h)</t>
   </si>
   <si>
-    <t>vref_mean</t>
-  </si>
-  <si>
-    <t>vref_std</t>
-  </si>
-  <si>
-    <t>vexp1_mean</t>
-  </si>
-  <si>
-    <t>vexp1_std</t>
+    <t>MBo10_mean</t>
+  </si>
+  <si>
+    <t>MBo10_std</t>
+  </si>
+  <si>
+    <t>MBo10_mean2</t>
+  </si>
+  <si>
+    <t>MBo10_std2</t>
   </si>
   <si>
     <t>enzyme/rxn</t>
@@ -562,7 +562,7 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D2:D7 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -694,8 +694,8 @@
   </sheetPr>
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D2:D7 A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -703,7 +703,7 @@
     <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>97</v>
       </c>
@@ -841,7 +841,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D2:D7 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1064,7 +1064,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D2:D7 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1384,15 +1384,15 @@
   </sheetPr>
   <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2:D7"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D2" activeCellId="1" sqref="A1:E1 D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.2591093117409"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.251012145749"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.3522267206478"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.4251012145749"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -1728,7 +1728,7 @@
   <dimension ref="A1:U14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D2:D7 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2665,7 +2665,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D2:D7 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3049,7 +3049,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D2:D7 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3272,7 +3272,7 @@
   <dimension ref="A2:A15"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D2:D7 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3369,7 +3369,7 @@
   <dimension ref="A2:A22"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D2:D7 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3501,7 +3501,7 @@
   <dimension ref="A2:A22"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D2:D7 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3633,7 +3633,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="D2:D7 B2"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="A1:E1 B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3814,7 +3814,7 @@
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E17" activeCellId="1" sqref="D2:D7 E17"/>
+      <selection pane="topLeft" activeCell="E17" activeCellId="1" sqref="A1:E1 E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Chore: updated measRates column names to work with new file format
</commit_message>
<xml_diff>
--- a/set_up_grasp_models/tests/test_files/test_check_models/HMP2360_r0_t0.xlsx
+++ b/set_up_grasp_models/tests/test_files/test_check_models/HMP2360_r0_t0.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="12"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="1" state="visible" r:id="rId2"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="134">
   <si>
     <t>General Reaction and Sampling Platform (GRASP)</t>
   </si>
@@ -325,19 +325,13 @@
     <t>max (M)</t>
   </si>
   <si>
-    <t>Fluxes (umol/gCDW/h)</t>
-  </si>
-  <si>
-    <t>MBo10_mean</t>
-  </si>
-  <si>
-    <t>MBo10_std</t>
-  </si>
-  <si>
-    <t>MBo10_mean2</t>
-  </si>
-  <si>
-    <t>MBo10_std2</t>
+    <t>reaction ID</t>
+  </si>
+  <si>
+    <t>vref_mean (umol/gCDW/h)</t>
+  </si>
+  <si>
+    <t>vref_std (umol/gCDW/h)</t>
   </si>
   <si>
     <t>enzyme/rxn</t>
@@ -356,9 +350,6 @@
   </si>
   <si>
     <t>MBo10_UB2 (M)</t>
-  </si>
-  <si>
-    <t>reaction ID</t>
   </si>
   <si>
     <t>kinetic mechanism</t>
@@ -574,7 +565,7 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:K1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -706,8 +697,8 @@
   </sheetPr>
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:K1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -726,10 +717,10 @@
         <v>99</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -853,7 +844,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:K1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -863,16 +854,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>103</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1076,7 +1067,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:K1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1089,13 +1080,13 @@
         <v>91</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1396,54 +1387,54 @@
   </sheetPr>
   <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:K1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.4574898785425"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.6356275303644"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.6720647773279"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.0647773279352"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="L1" s="1" t="s">
         <v>116</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1451,13 +1442,13 @@
         <v>39</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="F2" s="0" t="s">
         <v>24</v>
@@ -1469,7 +1460,7 @@
         <v>4</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1477,16 +1468,16 @@
         <v>40</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="J3" s="0" t="n">
         <v>0</v>
@@ -1495,7 +1486,7 @@
         <v>2</v>
       </c>
       <c r="L3" s="0" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1503,16 +1494,16 @@
         <v>41</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="F4" s="0" t="s">
         <v>27</v>
@@ -1524,7 +1515,7 @@
         <v>1</v>
       </c>
       <c r="L4" s="0" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1532,13 +1523,13 @@
         <v>42</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="J5" s="0" t="n">
         <v>0</v>
@@ -1547,7 +1538,7 @@
         <v>2</v>
       </c>
       <c r="L5" s="0" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1555,16 +1546,16 @@
         <v>43</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="J6" s="0" t="n">
         <v>0</v>
@@ -1573,7 +1564,7 @@
         <v>2</v>
       </c>
       <c r="L6" s="0" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1581,16 +1572,16 @@
         <v>44</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="F7" s="0" t="s">
         <v>27</v>
@@ -1602,7 +1593,7 @@
         <v>1</v>
       </c>
       <c r="L7" s="0" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1610,7 +1601,7 @@
         <v>45</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="J8" s="0" t="n">
         <v>0</v>
@@ -1624,7 +1615,7 @@
         <v>46</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="J9" s="0" t="n">
         <v>0</v>
@@ -1633,7 +1624,7 @@
         <v>1</v>
       </c>
       <c r="L9" s="0" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1641,7 +1632,7 @@
         <v>47</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="J10" s="0" t="n">
         <v>0</v>
@@ -1650,7 +1641,7 @@
         <v>1</v>
       </c>
       <c r="L10" s="0" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1658,7 +1649,7 @@
         <v>48</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="J11" s="0" t="n">
         <v>0</v>
@@ -1667,7 +1658,7 @@
         <v>1</v>
       </c>
       <c r="L11" s="0" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1675,7 +1666,7 @@
         <v>49</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="J12" s="0" t="n">
         <v>0</v>
@@ -1684,7 +1675,7 @@
         <v>1</v>
       </c>
       <c r="L12" s="0" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1692,7 +1683,7 @@
         <v>50</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="J13" s="0" t="n">
         <v>0</v>
@@ -1701,7 +1692,7 @@
         <v>1</v>
       </c>
       <c r="L13" s="0" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1709,7 +1700,7 @@
         <v>51</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="J14" s="0" t="n">
         <v>0</v>
@@ -1718,7 +1709,7 @@
         <v>1</v>
       </c>
       <c r="L14" s="0" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>
@@ -1740,7 +1731,7 @@
   <dimension ref="A1:U14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:K1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2677,7 +2668,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:K1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3061,7 +3052,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:K1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3284,7 +3275,7 @@
   <dimension ref="A2:A15"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:K1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3381,7 +3372,7 @@
   <dimension ref="A2:A22"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:K1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3513,7 +3504,7 @@
   <dimension ref="A2:A22"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:K1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3645,7 +3636,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="A1:K1 B2"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="A1:C1 B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3826,7 +3817,7 @@
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E17" activeCellId="1" sqref="A1:K1 E17"/>
+      <selection pane="topLeft" activeCell="E17" activeCellId="1" sqref="A1:C1 E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Feat: updated column names
</commit_message>
<xml_diff>
--- a/set_up_grasp_models/tests/test_files/test_check_models/HMP2360_r0_t0.xlsx
+++ b/set_up_grasp_models/tests/test_files/test_check_models/HMP2360_r0_t0.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="9"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="1" state="visible" r:id="rId2"/>
@@ -34,406 +34,406 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="134">
   <si>
-    <t>General Reaction and Sampling Platform (GRASP)</t>
-  </si>
-  <si>
-    <t>Unnamed: 1</t>
-  </si>
-  <si>
-    <t>Model name</t>
-  </si>
-  <si>
-    <t>HMP2360_r0_t0_promiscuous</t>
-  </si>
-  <si>
-    <t>Sampling mode (ORACLE, rejection, rejectionSMC, SMC, MCMC-SMC)</t>
-  </si>
-  <si>
-    <t>ORACLE</t>
-  </si>
-  <si>
-    <t>NLP solver (NLOPT, OPTI, FMINCON (default))</t>
-  </si>
-  <si>
-    <t>FMINCON</t>
-  </si>
-  <si>
-    <t>Number of exp. conditions (excluding reference state)</t>
-  </si>
-  <si>
-    <t>Number of model structures</t>
-  </si>
-  <si>
-    <t>Number of particles</t>
-  </si>
-  <si>
-    <t>Parallel mode (ON = 1; OFF = 0)</t>
-  </si>
-  <si>
-    <t>Number of cores (ignored if Parallel mode disabled)</t>
-  </si>
-  <si>
-    <t>Percentile of alive particles for SMC (e.g., 20, 50, etc.) (only needed for rejectionSMC, SMC, MCMC-SMC)</t>
-  </si>
-  <si>
-    <t>Compute robust fluxes (ON = 1; OFF = 0)</t>
-  </si>
-  <si>
-    <t>Compute thermodynamics (ON = 1; OFF = 0)</t>
-  </si>
-  <si>
-    <t>Inicial tolerance (OPTIONAL)</t>
-  </si>
-  <si>
-    <t>Final tolerance (in the case of ORACLE, set to 1)</t>
-  </si>
-  <si>
-    <t>rxn ID</t>
-  </si>
-  <si>
-    <t>accoa_c</t>
-  </si>
-  <si>
-    <t>sam_c</t>
-  </si>
-  <si>
-    <t>pterin1_c</t>
-  </si>
-  <si>
-    <t>trp_v</t>
-  </si>
-  <si>
-    <t>fivehtp_c</t>
-  </si>
-  <si>
-    <t>trp_c</t>
-  </si>
-  <si>
-    <t>srtn_c</t>
-  </si>
-  <si>
-    <t>nactsertn_c</t>
-  </si>
-  <si>
-    <t>meltn_c</t>
-  </si>
-  <si>
-    <t>tryptm_c</t>
-  </si>
-  <si>
-    <t>nactryptm_c</t>
-  </si>
-  <si>
-    <t>coa_c</t>
-  </si>
-  <si>
-    <t>sah_c</t>
-  </si>
-  <si>
-    <t>pterin2_c</t>
-  </si>
-  <si>
-    <t>fivehtp_e</t>
-  </si>
-  <si>
-    <t>trp_e</t>
-  </si>
-  <si>
-    <t>nactsertn_e</t>
-  </si>
-  <si>
-    <t>nactryptm_e</t>
-  </si>
-  <si>
-    <t>meltn_e</t>
-  </si>
-  <si>
-    <t>srtn_e</t>
-  </si>
-  <si>
-    <t>TPH</t>
-  </si>
-  <si>
-    <t>DDC</t>
-  </si>
-  <si>
-    <t>AANAT</t>
-  </si>
-  <si>
-    <t>ASMT</t>
-  </si>
-  <si>
-    <t>DDC_tryptm</t>
-  </si>
-  <si>
-    <t>AANAT_tryptm</t>
-  </si>
-  <si>
-    <t>IN_trp</t>
-  </si>
-  <si>
-    <t>EX_trp</t>
-  </si>
-  <si>
-    <t>EX_srtn</t>
-  </si>
-  <si>
-    <t>EX_fivehtp</t>
-  </si>
-  <si>
-    <t>EX_nactsertn</t>
-  </si>
-  <si>
-    <t>EX_meltn</t>
-  </si>
-  <si>
-    <t>EX_nactryptm</t>
-  </si>
-  <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>Metabolite name</t>
-  </si>
-  <si>
-    <t>balanced?</t>
-  </si>
-  <si>
-    <t>active?</t>
-  </si>
-  <si>
-    <t>fixed?</t>
-  </si>
-  <si>
-    <t>Acetyl-coa</t>
-  </si>
-  <si>
-    <t>S-adenosyl-methionine</t>
-  </si>
-  <si>
-    <t>tetrahydropterin</t>
-  </si>
-  <si>
-    <t>tryptophan produced by the cell</t>
-  </si>
-  <si>
-    <t>5-hydroxytryptophan</t>
-  </si>
-  <si>
-    <t>tryptophan</t>
-  </si>
-  <si>
-    <t>serotonin</t>
-  </si>
-  <si>
-    <t>N-acetylserotonin</t>
-  </si>
-  <si>
-    <t>melatonin</t>
-  </si>
-  <si>
-    <t>tryptamine</t>
-  </si>
-  <si>
-    <t>N-acetyltryptamine</t>
-  </si>
-  <si>
-    <t>coa</t>
-  </si>
-  <si>
-    <t>S-adenosyl-homocysteine</t>
-  </si>
-  <si>
-    <t>pterin-4a-carbinolamin</t>
-  </si>
-  <si>
-    <t>5-hydroxytryptophan external</t>
-  </si>
-  <si>
-    <t>tryptophan external</t>
-  </si>
-  <si>
-    <t>N-acetylserotonin external</t>
-  </si>
-  <si>
-    <t>N-acetyltryptamine external</t>
-  </si>
-  <si>
-    <t>melatonin external</t>
-  </si>
-  <si>
-    <t>serotonin external</t>
-  </si>
-  <si>
-    <t>reaction name</t>
-  </si>
-  <si>
-    <t>transportRxn?</t>
-  </si>
-  <si>
-    <t>modelled?</t>
-  </si>
-  <si>
-    <t>tryptophan hydroxylase</t>
-  </si>
-  <si>
-    <t>tryptophan decarboxylase</t>
-  </si>
-  <si>
-    <t>aralkylamine N-acetyltransferase</t>
-  </si>
-  <si>
-    <t>acetylserotonin methyltransferase</t>
-  </si>
-  <si>
-    <t>production of tryptophan by the cell</t>
-  </si>
-  <si>
-    <t>exchange tryptophan</t>
-  </si>
-  <si>
-    <t>exchange serotonin</t>
-  </si>
-  <si>
-    <t>Exchange 5-hydroxytryptophan</t>
-  </si>
-  <si>
-    <t>exchange n-acetylserotonin</t>
-  </si>
-  <si>
-    <t>exchange melatonin</t>
-  </si>
-  <si>
-    <t>exchange n-acetyltryptamin</t>
-  </si>
-  <si>
-    <t>met</t>
-  </si>
-  <si>
-    <t>rxn</t>
-  </si>
-  <si>
-    <t>∆Gr'_min (kJ/mol)</t>
-  </si>
-  <si>
-    <t>∆Gr'_max (kJ/mol)</t>
-  </si>
-  <si>
-    <t>min (M)</t>
-  </si>
-  <si>
-    <t>max (M)</t>
-  </si>
-  <si>
-    <t>reaction ID</t>
-  </si>
-  <si>
-    <t>vref_mean (umol/gCDW/h)</t>
-  </si>
-  <si>
-    <t>vref_std (umol/gCDW/h)</t>
-  </si>
-  <si>
-    <t>enzyme/rxn</t>
-  </si>
-  <si>
-    <t>MBo10_LB2</t>
-  </si>
-  <si>
-    <t>MBo10_meas2</t>
-  </si>
-  <si>
-    <t>MBo10_UB2</t>
-  </si>
-  <si>
-    <t>MBo10_LB2 (M)</t>
-  </si>
-  <si>
-    <t>MBo10_UB2 (M)</t>
-  </si>
-  <si>
-    <t>kinetic mechanism</t>
-  </si>
-  <si>
-    <t>substrate order</t>
-  </si>
-  <si>
-    <t>product order</t>
-  </si>
-  <si>
-    <t>promiscuous</t>
-  </si>
-  <si>
-    <t>inhibitors</t>
-  </si>
-  <si>
-    <t>activators</t>
-  </si>
-  <si>
-    <t>negative effectors</t>
-  </si>
-  <si>
-    <t>positive effectors</t>
-  </si>
-  <si>
-    <t>allosteric</t>
-  </si>
-  <si>
-    <t>subunits</t>
-  </si>
-  <si>
-    <t>comments</t>
-  </si>
-  <si>
-    <t>substrateInhibOrderedBiBi</t>
-  </si>
-  <si>
-    <t>pterin1_c trp_c trp_c fivehtp_c pterin2_c</t>
-  </si>
-  <si>
-    <t>putative homotetramer (metacyc). From pdb, might actually be a monomer. Tryptophan is substate inhibitor</t>
-  </si>
-  <si>
-    <t>UniUniPromiscuous</t>
-  </si>
-  <si>
-    <t>fivehtp_c trp_c srtn_c tryptm_c</t>
-  </si>
-  <si>
-    <t>DDC DDC_tryptm</t>
-  </si>
-  <si>
-    <t>homodimer (metacyc), inhib by serotonin</t>
-  </si>
-  <si>
-    <t>AANATCompInhibIndep</t>
-  </si>
-  <si>
-    <t>accoa_c srtn_c accoa_c tryptm_c meltn_c nactsertn_c nactryptm_c coa_c coa_c</t>
-  </si>
-  <si>
-    <t>AANAT AANAT_tryptm</t>
-  </si>
-  <si>
-    <t>Serotonin N-acetyltransferase is a monomeric enzyme (metacyc)</t>
-  </si>
-  <si>
-    <t>orderedBiBi</t>
-  </si>
-  <si>
-    <t>sam_c nactsertn_c meltn_c sah_c</t>
-  </si>
-  <si>
-    <t>ASMT has a C-terminal domain similar to other SAM-dependent O-methyltransferases, and an N-terminal domain which intertwines with another monomer to form the physiologically active dimer  (metacyc); inhib by melatonin</t>
-  </si>
-  <si>
-    <t>Serotonin N-acetyltransferase is a monomeric enzyme (metacyc); inhib by melatonin</t>
-  </si>
-  <si>
-    <t>massAction</t>
-  </si>
-  <si>
-    <t>Modeled as mass action</t>
+    <t xml:space="preserve">General Reaction and Sampling Platform (GRASP)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unnamed: 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Model name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HMP2360_r0_t0_promiscuous</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sampling mode (ORACLE, rejection, rejectionSMC, SMC, MCMC-SMC)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ORACLE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NLP solver (NLOPT, OPTI, FMINCON (default))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FMINCON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of exp. conditions (excluding reference state)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of model structures</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of particles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parallel mode (ON = 1; OFF = 0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of cores (ignored if Parallel mode disabled)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Percentile of alive particles for SMC (e.g., 20, 50, etc.) (only needed for rejectionSMC, SMC, MCMC-SMC)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Compute robust fluxes (ON = 1; OFF = 0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Compute thermodynamics (ON = 1; OFF = 0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inicial tolerance (OPTIONAL)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Final tolerance (in the case of ORACLE, set to 1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rxn ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">accoa_c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sam_c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pterin1_c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">trp_v</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fivehtp_c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">trp_c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">srtn_c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nactsertn_c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">meltn_c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tryptm_c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nactryptm_c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">coa_c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sah_c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pterin2_c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fivehtp_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">trp_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nactsertn_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nactryptm_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">meltn_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">srtn_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TPH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DDC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AANAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ASMT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DDC_tryptm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AANAT_tryptm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IN_trp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_trp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_srtn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_fivehtp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_nactsertn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_meltn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_nactryptm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Metabolite name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">balanced?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">active?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fixed?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Acetyl-coa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S-adenosyl-methionine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tetrahydropterin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tryptophan produced by the cell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5-hydroxytryptophan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tryptophan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">serotonin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N-acetylserotonin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">melatonin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tryptamine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N-acetyltryptamine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">coa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S-adenosyl-homocysteine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pterin-4a-carbinolamin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5-hydroxytryptophan external</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tryptophan external</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N-acetylserotonin external</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N-acetyltryptamine external</t>
+  </si>
+  <si>
+    <t xml:space="preserve">melatonin external</t>
+  </si>
+  <si>
+    <t xml:space="preserve">serotonin external</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reaction name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">transportRxn?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">modelled?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tryptophan hydroxylase</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tryptophan decarboxylase</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aralkylamine N-acetyltransferase</t>
+  </si>
+  <si>
+    <t xml:space="preserve">acetylserotonin methyltransferase</t>
+  </si>
+  <si>
+    <t xml:space="preserve">production of tryptophan by the cell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">exchange tryptophan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">exchange serotonin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exchange 5-hydroxytryptophan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">exchange n-acetylserotonin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">exchange melatonin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">exchange n-acetyltryptamin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">met</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rxn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">∆Gr'_min (kJ/mol)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">∆Gr'_max (kJ/mol)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">min (M)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">max (M)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reaction ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vref_mean (mmol/L/h)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vref_std (mmol/L/h)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">enzyme/rxn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MBo10_LB2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MBo10_meas2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MBo10_UB2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MBo10_LB2 (M)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MBo10_UB2 (M)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kinetic mechanism</t>
+  </si>
+  <si>
+    <t xml:space="preserve">substrate order</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product order</t>
+  </si>
+  <si>
+    <t xml:space="preserve">promiscuous</t>
+  </si>
+  <si>
+    <t xml:space="preserve">inhibitors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">activators</t>
+  </si>
+  <si>
+    <t xml:space="preserve">negative effectors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">positive effectors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">allosteric</t>
+  </si>
+  <si>
+    <t xml:space="preserve">subunits</t>
+  </si>
+  <si>
+    <t xml:space="preserve">comments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">substrateInhibOrderedBiBi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pterin1_c trp_c trp_c fivehtp_c pterin2_c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">putative homotetramer (metacyc). From pdb, might actually be a monomer. Tryptophan is substate inhibitor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UniUniPromiscuous</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fivehtp_c trp_c srtn_c tryptm_c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DDC DDC_tryptm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">homodimer (metacyc), inhib by serotonin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AANATCompInhibIndep</t>
+  </si>
+  <si>
+    <t xml:space="preserve">accoa_c srtn_c accoa_c tryptm_c meltn_c nactsertn_c nactryptm_c coa_c coa_c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AANAT AANAT_tryptm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Serotonin N-acetyltransferase is a monomeric enzyme (metacyc)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">orderedBiBi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sam_c nactsertn_c meltn_c sah_c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ASMT has a C-terminal domain similar to other SAM-dependent O-methyltransferases, and an N-terminal domain which intertwines with another monomer to form the physiologically active dimer  (metacyc); inhib by melatonin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Serotonin N-acetyltransferase is a monomeric enzyme (metacyc); inhib by melatonin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">massAction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Modeled as mass action</t>
   </si>
 </sst>
 </file>
@@ -441,7 +441,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -564,13 +564,13 @@
   </sheetPr>
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:C1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.57085020242915"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -682,7 +682,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -697,13 +697,13 @@
   </sheetPr>
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:C1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.57085020242915"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -828,7 +828,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -843,13 +843,13 @@
   </sheetPr>
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:C1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.57085020242915"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1051,7 +1051,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1066,13 +1066,13 @@
   </sheetPr>
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:C1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.57085020242915"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1372,7 +1372,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1387,16 +1387,16 @@
   </sheetPr>
   <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:C1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.6720647773279"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.0647773279352"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="8.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="25.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="8.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1715,7 +1715,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1730,13 +1730,13 @@
   </sheetPr>
   <dimension ref="A1:U14"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:C1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.57085020242915"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2652,7 +2652,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2667,13 +2667,13 @@
   </sheetPr>
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:C1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.57085020242915"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3036,7 +3036,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -3051,13 +3051,13 @@
   </sheetPr>
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:C1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.57085020242915"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3259,7 +3259,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -3274,13 +3274,13 @@
   </sheetPr>
   <dimension ref="A2:A15"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:C1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.57085020242915"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.57"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3356,7 +3356,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -3371,13 +3371,13 @@
   </sheetPr>
   <dimension ref="A2:A22"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:C1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.57085020242915"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.57"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3488,7 +3488,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -3503,13 +3503,13 @@
   </sheetPr>
   <dimension ref="A2:A22"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:C1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.57085020242915"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.57"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3620,7 +3620,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -3635,13 +3635,13 @@
   </sheetPr>
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="A1:C1 B2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="A1:E1 B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.57085020242915"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3801,7 +3801,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -3816,13 +3816,13 @@
   </sheetPr>
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E17" activeCellId="1" sqref="A1:C1 E17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E17" activeCellId="1" sqref="A1:E1 E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.57085020242915"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4059,7 +4059,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
tests: Update tests for new base file (general sheet)
</commit_message>
<xml_diff>
--- a/set_up_grasp_models/tests/test_files/test_check_models/HMP2360_r0_t0.xlsx
+++ b/set_up_grasp_models/tests/test_files/test_check_models/HMP2360_r0_t0.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="11"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="1" state="visible" r:id="rId2"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="125">
   <si>
     <t xml:space="preserve">General Reaction and Sampling Platform (GRASP)</t>
   </si>
@@ -45,7 +45,7 @@
     <t xml:space="preserve">Sampling mode (GRASP or rejection)</t>
   </si>
   <si>
-    <t xml:space="preserve">ORACLE</t>
+    <t xml:space="preserve">GRASP</t>
   </si>
   <si>
     <t xml:space="preserve">NLP solver (NLOPT or FMINCON (default))</t>
@@ -60,6 +60,15 @@
     <t xml:space="preserve">gurobi</t>
   </si>
   <si>
+    <t xml:space="preserve">Prior distribution for fluxes (uniform or normal)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">normal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prior distribution for thermodynamic quantities (uniform or normal)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Number of exp. conditions (excluding reference state)</t>
   </si>
   <si>
@@ -324,19 +333,13 @@
     <t xml:space="preserve">enzyme/rxn</t>
   </si>
   <si>
-    <t xml:space="preserve">MBo10_LB2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MBo10_meas2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MBo10_UB2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MBo10_LB2 (M)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MBo10_UB2 (M)</t>
+    <t xml:space="preserve">lower_bound</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">upper_bound</t>
   </si>
   <si>
     <t xml:space="preserve">kinetic mechanism</t>
@@ -501,7 +504,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -514,6 +517,10 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -524,31 +531,30 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:B1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="L2:L17 A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="37.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="8.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -593,29 +599,29 @@
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="0" t="n">
-        <v>1</v>
+      <c r="B6" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>10</v>
-      </c>
-      <c r="B7" s="0" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B8" s="0" t="n">
-        <v>10000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>1</v>
@@ -623,15 +629,15 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B10" s="0" t="n">
-        <v>2</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>1</v>
@@ -639,14 +645,28 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B12" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -660,38 +680,35 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="L2:L17 A1"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.57"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>0.938105540546311</v>
@@ -705,7 +722,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>0.948692986021061</v>
@@ -719,7 +736,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>0.963822080137339</v>
@@ -733,7 +750,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>0.781513345189378</v>
@@ -747,7 +764,7 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>0.99</v>
@@ -761,7 +778,7 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>0.99</v>
@@ -775,7 +792,7 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>0.99</v>
@@ -789,7 +806,7 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>0.99</v>
@@ -803,7 +820,7 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>0.99</v>
@@ -817,7 +834,7 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>0.99</v>
@@ -831,7 +848,7 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>0.99</v>
@@ -845,7 +862,7 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>0.99</v>
@@ -859,7 +876,7 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>0.99</v>
@@ -883,38 +900,35 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="L2:L17 A1"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.57"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>100</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>0.600926593306472</v>
@@ -928,7 +942,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>0.99</v>
@@ -942,7 +956,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>0.99</v>
@@ -956,7 +970,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>0.99</v>
@@ -970,7 +984,7 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>0.99</v>
@@ -984,7 +998,7 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>0.897059063218122</v>
@@ -998,7 +1012,7 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>0.879431204670374</v>
@@ -1012,7 +1026,7 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>0.851303699101255</v>
@@ -1026,7 +1040,7 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>0.913109189061105</v>
@@ -1040,7 +1054,7 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>0.965053927008861</v>
@@ -1054,7 +1068,7 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>0.622035526990772</v>
@@ -1068,7 +1082,7 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>0.799696511562971</v>
@@ -1082,7 +1096,7 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>0.99</v>
@@ -1096,7 +1110,7 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>0.99</v>
@@ -1110,7 +1124,7 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>0.99</v>
@@ -1124,7 +1138,7 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>0.99</v>
@@ -1138,7 +1152,7 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>0.771228436522274</v>
@@ -1152,7 +1166,7 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>0.967924985045021</v>
@@ -1166,7 +1180,7 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>0.994407168746068</v>
@@ -1180,7 +1194,7 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>0.989083174460458</v>
@@ -1204,77 +1218,75 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L2" activeCellId="0" sqref="L2:L17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L2" activeCellId="0" sqref="L2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="8.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="25.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="8.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="C1" s="4" t="s">
+      <c r="A1" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="C1" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="D1" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="E1" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="F1" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="G1" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="H1" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="I1" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="J1" s="5" t="s">
         <v>111</v>
       </c>
+      <c r="K1" s="5" t="s">
+        <v>112</v>
+      </c>
       <c r="L1" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="J2" s="0" t="n">
         <v>0</v>
@@ -1285,19 +1297,19 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="J3" s="0" t="n">
         <v>0</v>
@@ -1308,22 +1320,22 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="J4" s="0" t="n">
         <v>0</v>
@@ -1334,16 +1346,16 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="J5" s="0" t="n">
         <v>0</v>
@@ -1354,19 +1366,19 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="J6" s="0" t="n">
         <v>0</v>
@@ -1377,22 +1389,22 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="J7" s="0" t="n">
         <v>0</v>
@@ -1403,10 +1415,10 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="J8" s="0" t="n">
         <v>0</v>
@@ -1417,10 +1429,10 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="J9" s="0" t="n">
         <v>0</v>
@@ -1431,10 +1443,10 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="J10" s="0" t="n">
         <v>0</v>
@@ -1445,10 +1457,10 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="J11" s="0" t="n">
         <v>0</v>
@@ -1459,10 +1471,10 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="J12" s="0" t="n">
         <v>0</v>
@@ -1473,10 +1485,10 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="J13" s="0" t="n">
         <v>0</v>
@@ -1487,10 +1499,10 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="J14" s="0" t="n">
         <v>0</v>
@@ -1511,89 +1523,86 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:U14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="L2:L17 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.57"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="S1" s="2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="T1" s="2" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="U1" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>0</v>
@@ -1658,7 +1667,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>0</v>
@@ -1723,7 +1732,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>-1</v>
@@ -1788,7 +1797,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>0</v>
@@ -1853,7 +1862,7 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>0</v>
@@ -1918,7 +1927,7 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>-1</v>
@@ -1983,7 +1992,7 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>0</v>
@@ -2048,7 +2057,7 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>0</v>
@@ -2113,7 +2122,7 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>0</v>
@@ -2178,7 +2187,7 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>0</v>
@@ -2243,7 +2252,7 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>0</v>
@@ -2308,7 +2317,7 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>0</v>
@@ -2373,7 +2382,7 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>0</v>
@@ -2448,39 +2457,38 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="1" sqref="L2:L17 D1"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1021" min="1" style="0" width="8.57"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1022" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1022" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>0</v>
@@ -2488,10 +2496,10 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>0</v>
@@ -2499,10 +2507,10 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>0</v>
@@ -2510,10 +2518,10 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>0</v>
@@ -2521,10 +2529,10 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>1</v>
@@ -2532,10 +2540,10 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>1</v>
@@ -2543,10 +2551,10 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>1</v>
@@ -2554,10 +2562,10 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>1</v>
@@ -2565,10 +2573,10 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>1</v>
@@ -2576,10 +2584,10 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>1</v>
@@ -2587,10 +2595,10 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>1</v>
@@ -2598,10 +2606,10 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>0</v>
@@ -2609,10 +2617,10 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>0</v>
@@ -2620,10 +2628,10 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>0</v>
@@ -2631,10 +2639,10 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>0</v>
@@ -2642,10 +2650,10 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>0</v>
@@ -2653,10 +2661,10 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="C18" s="0" t="n">
         <v>0</v>
@@ -2664,10 +2672,10 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="C19" s="0" t="n">
         <v>0</v>
@@ -2675,10 +2683,10 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C20" s="0" t="n">
         <v>0</v>
@@ -2686,10 +2694,10 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C21" s="0" t="n">
         <v>0</v>
@@ -2707,42 +2715,41 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="1" sqref="L2:L17 D1"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="1" style="0" width="8.57"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>75</v>
+        <v>77</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>0</v>
@@ -2750,10 +2757,10 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>0</v>
@@ -2761,10 +2768,10 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>0</v>
@@ -2772,10 +2779,10 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>0</v>
@@ -2783,10 +2790,10 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>0</v>
@@ -2794,10 +2801,10 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>0</v>
@@ -2805,10 +2812,10 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>0</v>
@@ -2816,10 +2823,10 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>0</v>
@@ -2827,10 +2834,10 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>0</v>
@@ -2838,10 +2845,10 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>0</v>
@@ -2849,10 +2856,10 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>0</v>
@@ -2860,10 +2867,10 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>0</v>
@@ -2871,10 +2878,10 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>0</v>
@@ -2892,124 +2899,121 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A2:A22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="L2:L17 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.57"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -3024,124 +3028,121 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A2:A22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="L2:L17 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.57"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -3156,35 +3157,32 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="L2:L17 B2"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.57"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>-60</v>
@@ -3195,7 +3193,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>-37.2</v>
@@ -3206,7 +3204,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>-50</v>
@@ -3217,7 +3215,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>-23.24</v>
@@ -3228,7 +3226,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>-43.2</v>
@@ -3239,7 +3237,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>-24.6</v>
@@ -3250,7 +3248,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>-40</v>
@@ -3261,7 +3259,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>-10</v>
@@ -3272,7 +3270,7 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>-30</v>
@@ -3283,7 +3281,7 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>-10</v>
@@ -3294,7 +3292,7 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>-10</v>
@@ -3305,7 +3303,7 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>-10</v>
@@ -3316,7 +3314,7 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>-10</v>
@@ -3337,35 +3335,32 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E17" activeCellId="1" sqref="L2:L17 E17"/>
+      <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.57"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>0.000228462011808056</v>
@@ -3376,7 +3371,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>1E-012</v>
@@ -3387,7 +3382,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>1E-012</v>
@@ -3398,7 +3393,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>1E-012</v>
@@ -3409,7 +3404,7 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>1E-012</v>
@@ -3420,7 +3415,7 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>0.00559675402823174</v>
@@ -3431,7 +3426,7 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>1E-012</v>
@@ -3442,7 +3437,7 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>0.00310804602125163</v>
@@ -3453,7 +3448,7 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>0.0308279171448426</v>
@@ -3464,7 +3459,7 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>0.00181042853161852</v>
@@ -3475,7 +3470,7 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>8.28736361429022E-005</v>
@@ -3486,7 +3481,7 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>0.00604381725975038</v>
@@ -3497,7 +3492,7 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>1E-012</v>
@@ -3508,7 +3503,7 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>1E-012</v>
@@ -3519,7 +3514,7 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>1E-012</v>
@@ -3530,7 +3525,7 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>1E-012</v>
@@ -3541,7 +3536,7 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>9.44630572239322E-006</v>
@@ -3552,7 +3547,7 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>5.16846874940607E-006</v>
@@ -3563,7 +3558,7 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>0.000856570953217132</v>
@@ -3574,7 +3569,7 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>0.00016291524956886</v>
@@ -3595,36 +3590,35 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="1" sqref="L2:L17 D1"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1022" min="1" style="0" width="8.57"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1023" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1023" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>-81.4547774583559</v>
@@ -3635,7 +3629,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>18.5183721041727</v>
@@ -3646,7 +3640,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>0.431738943043251</v>
@@ -3657,7 +3651,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>-0.567354685137039</v>
@@ -3668,7 +3662,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>85.3794767878033</v>
@@ -3679,7 +3673,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>0.103545682502924</v>

</xml_diff>